<commit_message>
Workable version for the test.py to find the valid result
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97738\Desktop\歼灭判断\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C752079B-F06E-417F-A69A-E05E5E322627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF58D9F0-6A36-463C-BCC5-CE1253D76FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{776165D5-EE0D-48F6-8A93-C47D3D25E7BC}"/>
+    <workbookView xWindow="32535" yWindow="5730" windowWidth="10560" windowHeight="11220" xr2:uid="{776165D5-EE0D-48F6-8A93-C47D3D25E7BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
[new-update] able to proceed known cases and unkown cases (by changing fron code at main.py
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,24 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97738\Desktop\歼灭判断\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97738\Desktop\call_me_DZG_judger_for_HuBiaoTasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E22A40F-9684-4EE9-837B-F31F18A2704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF3A6D0-2CB9-428F-93DB-C34F34E87BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="others" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="my-data" sheetId="1" r:id="rId1"/>
+    <sheet name="oldenemy" sheetId="2" r:id="rId2"/>
+    <sheet name="enemey-sanrenhe" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -79,13 +79,93 @@
   </si>
   <si>
     <t>卖伞女</t>
+  </si>
+  <si>
+    <t>草原女孩</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>苗疆</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>卖伞女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>书香女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>针线女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>绣娘</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>采药女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>琵琶女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>丫鬟</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>草原女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>将门女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>西域女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>棋士</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>捕快</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>迅鹰女</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>驯马师</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>花艺师</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>役使</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>李师师</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小师妹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +185,13 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -149,6 +236,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -456,8 +546,8 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -479,7 +569,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>1018</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -487,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>615</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -495,7 +585,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>550</v>
+        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -503,7 +593,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>400</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -511,7 +601,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>316</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -519,7 +609,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <v>268</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -527,7 +617,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -535,7 +625,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="3">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -543,7 +633,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -551,7 +641,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -567,7 +657,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="3">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -575,7 +665,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="3">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -583,7 +673,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="3">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -591,7 +681,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -607,7 +697,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -624,7 +714,9 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -734,9 +826,9 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="B10" s="3">
         <v>123</v>
@@ -804,17 +896,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" style="4" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,140 +912,156 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="3">
-        <v>100</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>2342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[minor-update] adjust main.py slightly
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97738\Desktop\call_me_DZG_judger_for_HuBiaoTasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF3A6D0-2CB9-428F-93DB-C34F34E87BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B452F7-ADD1-4ABF-9A83-A6D3B97338B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my-data" sheetId="1" r:id="rId1"/>
     <sheet name="oldenemy" sheetId="2" r:id="rId2"/>
-    <sheet name="enemey-sanrenhe" sheetId="3" r:id="rId3"/>
+    <sheet name="enemy-sanrenhe" sheetId="3" r:id="rId3"/>
+    <sheet name="enemy-shanhaiboring" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -158,6 +160,53 @@
   </si>
   <si>
     <t>小师妹</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>小乞丐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>红娘子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>医师</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>蒙琪儿</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>戏子</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>剑舞者</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>山海无情</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy-shanhaiboring</t>
+  </si>
+  <si>
+    <t>enemyName</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy-sheetname</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>三人禾</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy-sanrenhe</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -898,8 +947,8 @@
   </sheetPr>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1068,4 +1117,224 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96370C57-472B-4D3F-B6C8-2FAB15BDE5E9}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E446786-6D8D-47C9-8F02-2B87A1CB5266}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[nothing] adjust some data
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97738\Desktop\call_me_DZG_judger_for_HuBiaoTasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06480C0-4599-4C9A-9939-BAFD7DA8D92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC87E63C-2EB0-4A09-91C0-BFAE89E21D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="my-data" sheetId="1" r:id="rId1"/>
     <sheet name="oldenemy" sheetId="2" r:id="rId2"/>
     <sheet name="enemy-sanrenhe" sheetId="3" r:id="rId3"/>
     <sheet name="enemy-shanhaiboring" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
-    <sheet name="enemy-ruizedalang" sheetId="7" r:id="rId6"/>
+    <sheet name="enemy-wuyanzu" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
+    <sheet name="enemy-ruizedalang" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -228,6 +229,14 @@
   </si>
   <si>
     <t>陆长青</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>潇洒吴彦祖</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>enemy-wuyanzu</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -614,10 +623,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -626,7 +635,7 @@
     <col min="2" max="2" width="13.625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,72 +643,63 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3">
         <v>341</v>
       </c>
-      <c r="G6" s="3">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>307</v>
       </c>
-      <c r="G7" s="3">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>208</v>
       </c>
-      <c r="G8">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -707,7 +707,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -715,7 +715,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -723,7 +723,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -731,7 +731,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -739,7 +739,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -747,7 +747,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -755,7 +755,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1326,11 +1326,235 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81EA73D-6E41-49A0-A5BB-2BBE08ABFF1D}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26">
+        <v>99999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E446786-6D8D-47C9-8F02-2B87A1CB5266}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1371,18 +1595,26 @@
         <v>52</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1326C1B-0E86-4CCC-9A03-FD4D00691CF7}">
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="D43" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>